<commit_message>
Second commit, routed digital data inputs of DAC
Now I have problems routing the WRTA & WRTB pins of the DAC. Will probably have to reassign some pins of the digital data inputs (potential solution: I could make the WRTA/WRTB pair be situated at LA29, and the DAC_DB input pins would have to be cascaded down. DAC_DB1/DAC_DB0 would then have to be moved to the other side of the LPC connector, probably where WRTA/WRTB are now, at LA26). It'll look weird in the pinout diagram, but at least it'll work (hopefully :@    )
</commit_message>
<xml_diff>
--- a/VITA 57.4 LPC_ADCDAC_Pinout.xlsx
+++ b/VITA 57.4 LPC_ADCDAC_Pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TCFH2003\Documents\!!PCB_Projects\ML605_Virtex6_EvalBoard_ExpansionCards\ML605_LPC_Board_wADC_DAC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9BC6FF-ADBC-4A8E-BEC5-83B7227A292E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F101A95B-20F2-40A4-80B7-F25FCB0A000A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3AF5A803-F458-42AE-90A9-8BC82334C65E}"/>
   </bookViews>
@@ -527,9 +527,6 @@
     <t>DAC_DB6</t>
   </si>
   <si>
-    <t>DAC_DA7</t>
-  </si>
-  <si>
     <t>DAC_DB7</t>
   </si>
   <si>
@@ -612,6 +609,9 @@
   </si>
   <si>
     <t>PRSNT_M2C_L (GPIO)</t>
+  </si>
+  <si>
+    <t>DAC_DA2</t>
   </si>
 </sst>
 </file>
@@ -2576,8 +2576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DAE75D3-E98E-4002-BF12-A44E854FFC55}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4033,8 +4033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EBE69E-1DFC-4A9A-9239-DABE3059A25F}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4125,10 +4125,10 @@
         <v>106</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>106</v>
@@ -4163,7 +4163,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>106</v>
@@ -4195,7 +4195,7 @@
         <v>106</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
@@ -4230,7 +4230,7 @@
         <v>106</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>10</v>
@@ -4347,7 +4347,7 @@
         <v>106</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>10</v>
@@ -4382,7 +4382,7 @@
         <v>106</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>10</v>
@@ -4420,7 +4420,7 @@
         <v>10</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>106</v>
@@ -4452,10 +4452,10 @@
         <v>106</v>
       </c>
       <c r="H12" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="I12" s="10" t="s">
         <v>171</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>170</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>106</v>
@@ -4487,7 +4487,7 @@
         <v>106</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>10</v>
@@ -4557,10 +4557,10 @@
         <v>106</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>106</v>
@@ -4592,10 +4592,10 @@
         <v>106</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J16" s="19" t="s">
         <v>106</v>
@@ -4662,7 +4662,7 @@
         <v>106</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>10</v>
@@ -4697,10 +4697,10 @@
         <v>106</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>106</v>
@@ -4735,7 +4735,7 @@
         <v>10</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>106</v>
@@ -4767,7 +4767,7 @@
         <v>106</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>10</v>
@@ -4802,7 +4802,7 @@
         <v>106</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>10</v>
@@ -4840,7 +4840,7 @@
         <v>10</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J23" s="19" t="s">
         <v>106</v>
@@ -4872,10 +4872,10 @@
         <v>106</v>
       </c>
       <c r="H24" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="I24" s="10" t="s">
         <v>185</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>184</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>106</v>
@@ -4907,7 +4907,7 @@
         <v>106</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>10</v>
@@ -4977,10 +4977,10 @@
         <v>106</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>106</v>
@@ -5012,10 +5012,10 @@
         <v>106</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>188</v>
+        <v>148</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J28" s="19" t="s">
         <v>106</v>
@@ -5070,7 +5070,7 @@
         <v>106</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>10</v>
@@ -5108,7 +5108,7 @@
         <v>10</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F31" s="19" t="s">
         <v>106</v>
@@ -5140,10 +5140,10 @@
         <v>106</v>
       </c>
       <c r="D32" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E32" s="10" t="s">
         <v>167</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>168</v>
       </c>
       <c r="F32" s="19" t="s">
         <v>106</v>
@@ -5175,7 +5175,7 @@
         <v>106</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>10</v>
@@ -5213,7 +5213,7 @@
         <v>10</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>163</v>
+        <v>191</v>
       </c>
       <c r="F34" s="19" t="s">
         <v>106</v>
@@ -5245,10 +5245,10 @@
         <v>106</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F35" s="19" t="s">
         <v>106</v>
@@ -5280,7 +5280,7 @@
         <v>106</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>10</v>
@@ -5318,7 +5318,7 @@
         <v>10</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="F37" s="19" t="s">
         <v>106</v>
@@ -5350,10 +5350,10 @@
         <v>106</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="F38" s="19" t="s">
         <v>106</v>
@@ -5385,7 +5385,7 @@
         <v>106</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
The ADC/DAC part of the board is done
Now I just need to figure out how to do the GPIO breakout, but I have a lot more flexibility here. Ideally, I'd like to keep the PMOD connector format, however I'm not sure if that is going to be possible. If I can't do that due to routing issues, than I can probably just stick a 50-something pin header on the the top side of the board at the left edge, on the other side of the LPC connector and call it a day.
</commit_message>
<xml_diff>
--- a/VITA 57.4 LPC_ADCDAC_Pinout.xlsx
+++ b/VITA 57.4 LPC_ADCDAC_Pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TCFH2003\Documents\!!PCB_Projects\ML605_Virtex6_EvalBoard_ExpansionCards\ML605_LPC_Board_wADC_DAC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F101A95B-20F2-40A4-80B7-F25FCB0A000A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC274BE0-2AD9-4A35-B0D3-F896849D967F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3AF5A803-F458-42AE-90A9-8BC82334C65E}"/>
   </bookViews>
@@ -2576,8 +2576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DAE75D3-E98E-4002-BF12-A44E854FFC55}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4034,7 +4034,7 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4127,8 +4127,8 @@
       <c r="D3" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>109</v>
+      <c r="E3" s="10" t="s">
+        <v>168</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>106</v>
@@ -4162,8 +4162,8 @@
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>110</v>
+      <c r="E4" s="10" t="s">
+        <v>169</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>106</v>
@@ -4347,7 +4347,7 @@
         <v>106</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>10</v>
@@ -4382,7 +4382,7 @@
         <v>106</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>10</v>
@@ -4420,7 +4420,7 @@
         <v>10</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>106</v>
@@ -4452,10 +4452,10 @@
         <v>106</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>106</v>
@@ -4487,7 +4487,7 @@
         <v>106</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>10</v>
@@ -4557,10 +4557,10 @@
         <v>106</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>106</v>
@@ -4592,10 +4592,10 @@
         <v>106</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J16" s="19" t="s">
         <v>106</v>
@@ -4662,7 +4662,7 @@
         <v>106</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>10</v>
@@ -4697,10 +4697,10 @@
         <v>106</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>106</v>
@@ -4735,7 +4735,7 @@
         <v>10</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>106</v>
@@ -4767,7 +4767,7 @@
         <v>106</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>10</v>
@@ -4802,7 +4802,7 @@
         <v>106</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>10</v>
@@ -4840,7 +4840,7 @@
         <v>10</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="J23" s="19" t="s">
         <v>106</v>
@@ -4872,10 +4872,10 @@
         <v>106</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>106</v>
@@ -4898,7 +4898,7 @@
         <v>10</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F25" s="19" t="s">
         <v>106</v>
@@ -4907,7 +4907,7 @@
         <v>106</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>10</v>
@@ -4930,10 +4930,10 @@
         <v>106</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>106</v>
@@ -4965,7 +4965,7 @@
         <v>106</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>10</v>
@@ -4976,8 +4976,8 @@
       <c r="G27" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="H27" s="10" t="s">
-        <v>149</v>
+      <c r="H27" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>188</v>
@@ -5003,7 +5003,7 @@
         <v>10</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F28" s="19" t="s">
         <v>106</v>
@@ -5011,8 +5011,8 @@
       <c r="G28" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="H28" s="10" t="s">
-        <v>148</v>
+      <c r="H28" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>189</v>
@@ -5035,10 +5035,10 @@
         <v>106</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F29" s="19" t="s">
         <v>106</v>
@@ -5070,7 +5070,7 @@
         <v>106</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>10</v>
@@ -5108,7 +5108,7 @@
         <v>10</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="F31" s="19" t="s">
         <v>106</v>
@@ -5143,7 +5143,7 @@
         <v>150</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="F32" s="19" t="s">
         <v>106</v>

</xml_diff>

<commit_message>
Review photos and Mezzaninne spelling mistake fixed
</commit_message>
<xml_diff>
--- a/VITA 57.4 LPC_ADCDAC_Pinout.xlsx
+++ b/VITA 57.4 LPC_ADCDAC_Pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TCFH2003\Documents\!!PCB_Projects\ML605_Virtex6_EvalBoard_ExpansionCards\ML605_LPC_Board_wADC_DAC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4099D8C-4B54-4713-90EE-79AEB7109B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB46330-1415-4B89-AC0B-235EBF36809D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3AF5A803-F458-42AE-90A9-8BC82334C65E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3AF5A803-F458-42AE-90A9-8BC82334C65E}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 5-1 LPC" sheetId="3" r:id="rId1"/>
@@ -365,12 +365,6 @@
     <t>ADC_CLK_N (40MHz)</t>
   </si>
   <si>
-    <t>DAC_CLK_P (100MHz)</t>
-  </si>
-  <si>
-    <t>DAC_CLK_N (100MHz)</t>
-  </si>
-  <si>
     <t>ADC_I0</t>
   </si>
   <si>
@@ -612,6 +606,12 @@
   </si>
   <si>
     <t>DAC_DA2</t>
+  </si>
+  <si>
+    <t>DAC_CLK_P (200MHz)</t>
+  </si>
+  <si>
+    <t>DAC_CLK_N (200MHz)</t>
   </si>
 </sst>
 </file>
@@ -929,7 +929,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="609600" y="0"/>
+          <a:off x="605118" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -1081,7 +1081,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3581400" y="0"/>
+          <a:off x="3585882" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -1157,7 +1157,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5067300" y="0"/>
+          <a:off x="5076265" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -1233,7 +1233,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6553200" y="0"/>
+          <a:off x="6566647" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -1309,7 +1309,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9525000" y="0"/>
+          <a:off x="9547412" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -1385,7 +1385,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11010900" y="0"/>
+          <a:off x="11037794" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -1461,7 +1461,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12496800" y="0"/>
+          <a:off x="12528176" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -1537,7 +1537,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="13982700" y="0"/>
+          <a:off x="14018559" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -1618,7 +1618,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="609600" y="0"/>
+          <a:off x="605118" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -1770,7 +1770,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3581400" y="0"/>
+          <a:off x="3585882" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -1846,7 +1846,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5067300" y="0"/>
+          <a:off x="5076265" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -1922,7 +1922,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6553200" y="0"/>
+          <a:off x="6566647" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -1998,7 +1998,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9525000" y="0"/>
+          <a:off x="9547412" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -2074,7 +2074,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11010900" y="0"/>
+          <a:off x="11037794" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -2150,7 +2150,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12496800" y="0"/>
+          <a:off x="12528176" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -2226,7 +2226,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="13982700" y="0"/>
+          <a:off x="14018559" y="0"/>
           <a:ext cx="2540" cy="2540"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="4" cy="4"/>
@@ -2576,7 +2576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DAE75D3-E98E-4002-BF12-A44E854FFC55}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -4033,8 +4033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EBE69E-1DFC-4A9A-9239-DABE3059A25F}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4090,7 +4090,7 @@
         <v>106</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>10</v>
@@ -4102,7 +4102,7 @@
         <v>106</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>10</v>
@@ -4125,10 +4125,10 @@
         <v>106</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>106</v>
@@ -4140,7 +4140,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J3" s="19" t="s">
         <v>106</v>
@@ -4163,7 +4163,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>106</v>
@@ -4175,7 +4175,7 @@
         <v>10</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J4" s="19" t="s">
         <v>106</v>
@@ -4207,7 +4207,7 @@
         <v>106</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>10</v>
@@ -4242,7 +4242,7 @@
         <v>106</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>10</v>
@@ -4268,7 +4268,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>106</v>
@@ -4280,7 +4280,7 @@
         <v>10</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J7" s="19" t="s">
         <v>106</v>
@@ -4300,10 +4300,10 @@
         <v>106</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F8" s="19" t="s">
         <v>106</v>
@@ -4315,7 +4315,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J8" s="19" t="s">
         <v>106</v>
@@ -4335,7 +4335,7 @@
         <v>106</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>10</v>
@@ -4347,7 +4347,7 @@
         <v>106</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>10</v>
@@ -4373,7 +4373,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>106</v>
@@ -4382,7 +4382,7 @@
         <v>106</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>10</v>
@@ -4405,11 +4405,11 @@
         <v>106</v>
       </c>
       <c r="D11" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>130</v>
-      </c>
       <c r="F11" s="19" t="s">
         <v>106</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>10</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>106</v>
@@ -4440,7 +4440,7 @@
         <v>106</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>10</v>
@@ -4452,10 +4452,10 @@
         <v>106</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>106</v>
@@ -4478,7 +4478,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>106</v>
@@ -4487,7 +4487,7 @@
         <v>106</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>10</v>
@@ -4510,10 +4510,10 @@
         <v>106</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>122</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>106</v>
@@ -4545,7 +4545,7 @@
         <v>106</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>10</v>
@@ -4557,10 +4557,10 @@
         <v>106</v>
       </c>
       <c r="H15" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="I15" s="10" t="s">
         <v>176</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>178</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>106</v>
@@ -4583,7 +4583,7 @@
         <v>10</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>106</v>
@@ -4592,10 +4592,10 @@
         <v>106</v>
       </c>
       <c r="H16" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="I16" s="10" t="s">
         <v>177</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>179</v>
       </c>
       <c r="J16" s="19" t="s">
         <v>106</v>
@@ -4615,10 +4615,10 @@
         <v>106</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F17" s="19" t="s">
         <v>106</v>
@@ -4650,7 +4650,7 @@
         <v>106</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>10</v>
@@ -4662,7 +4662,7 @@
         <v>106</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>10</v>
@@ -4688,7 +4688,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F19" s="19" t="s">
         <v>106</v>
@@ -4697,10 +4697,10 @@
         <v>106</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>106</v>
@@ -4720,11 +4720,11 @@
         <v>106</v>
       </c>
       <c r="D20" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>125</v>
-      </c>
       <c r="F20" s="19" t="s">
         <v>106</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>10</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>106</v>
@@ -4755,7 +4755,7 @@
         <v>106</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>10</v>
@@ -4767,7 +4767,7 @@
         <v>106</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>10</v>
@@ -4793,7 +4793,7 @@
         <v>10</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F22" s="19" t="s">
         <v>106</v>
@@ -4802,7 +4802,7 @@
         <v>106</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>10</v>
@@ -4825,11 +4825,11 @@
         <v>106</v>
       </c>
       <c r="D23" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>117</v>
-      </c>
       <c r="F23" s="19" t="s">
         <v>106</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>10</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J23" s="19" t="s">
         <v>106</v>
@@ -4860,7 +4860,7 @@
         <v>106</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>10</v>
@@ -4872,10 +4872,10 @@
         <v>106</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>106</v>
@@ -4898,7 +4898,7 @@
         <v>10</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F25" s="19" t="s">
         <v>106</v>
@@ -4907,7 +4907,7 @@
         <v>106</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>10</v>
@@ -4930,10 +4930,10 @@
         <v>106</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>106</v>
@@ -4965,7 +4965,7 @@
         <v>106</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>10</v>
@@ -4977,10 +4977,10 @@
         <v>106</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>106</v>
@@ -5003,7 +5003,7 @@
         <v>10</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F28" s="19" t="s">
         <v>106</v>
@@ -5012,10 +5012,10 @@
         <v>106</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J28" s="19" t="s">
         <v>106</v>
@@ -5035,10 +5035,10 @@
         <v>106</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F29" s="19" t="s">
         <v>106</v>
@@ -5070,7 +5070,7 @@
         <v>106</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>10</v>
@@ -5082,7 +5082,7 @@
         <v>106</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>10</v>
@@ -5108,7 +5108,7 @@
         <v>10</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F31" s="19" t="s">
         <v>106</v>
@@ -5117,10 +5117,10 @@
         <v>106</v>
       </c>
       <c r="H31" s="22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J31" s="19" t="s">
         <v>106</v>
@@ -5140,10 +5140,10 @@
         <v>106</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F32" s="19" t="s">
         <v>106</v>
@@ -5152,10 +5152,10 @@
         <v>106</v>
       </c>
       <c r="H32" s="22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J32" s="19" t="s">
         <v>106</v>
@@ -5175,7 +5175,7 @@
         <v>106</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>10</v>
@@ -5213,7 +5213,7 @@
         <v>10</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F34" s="19" t="s">
         <v>106</v>
@@ -5222,7 +5222,7 @@
         <v>106</v>
       </c>
       <c r="H34" s="22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I34" s="5" t="s">
         <v>10</v>
@@ -5245,10 +5245,10 @@
         <v>106</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F35" s="19" t="s">
         <v>106</v>
@@ -5257,10 +5257,10 @@
         <v>106</v>
       </c>
       <c r="H35" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="I35" s="22" t="s">
         <v>135</v>
-      </c>
-      <c r="I35" s="22" t="s">
-        <v>137</v>
       </c>
       <c r="J35" s="19" t="s">
         <v>106</v>
@@ -5280,7 +5280,7 @@
         <v>106</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>10</v>
@@ -5292,7 +5292,7 @@
         <v>106</v>
       </c>
       <c r="H36" s="22" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I36" s="12" t="s">
         <v>98</v>
@@ -5318,7 +5318,7 @@
         <v>10</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F37" s="19" t="s">
         <v>106</v>
@@ -5350,10 +5350,10 @@
         <v>106</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F38" s="19" t="s">
         <v>106</v>
@@ -5385,7 +5385,7 @@
         <v>106</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>10</v>
@@ -5481,12 +5481,12 @@
     </row>
     <row r="45" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G45" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G46" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>